<commit_message>
Finition des contrôleurs et des vues
</commit_message>
<xml_diff>
--- a/docs/Analysis/RP_Planification.xlsx
+++ b/docs/Analysis/RP_Planification.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11730" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11280" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Prévisionnel" sheetId="1" r:id="rId1"/>
@@ -442,7 +442,40 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="61">
+  <dxfs count="65">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1183,8 +1216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N47"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2399,101 +2432,101 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:M2 F43:F44 H43:I44 I32:I42 C3:C30 I3:I30 L3:L30 E23:E24 E26:E30 F25 G3:G30 E3:E18 F19:F21 I45 C32:C45 E32:E45 G32:G45 L32:L45">
-    <cfRule type="cellIs" dxfId="60" priority="38" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="64" priority="38" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:M2 C23:M24 C32:M45 C4:M18 C26:M30 C25:D25 F25:M25 C19:D21 F19:M21 K31:M31 I31">
-    <cfRule type="cellIs" dxfId="59" priority="37" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="63" priority="37" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L40 I40 G40 E40 C40">
-    <cfRule type="cellIs" dxfId="58" priority="36" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="62" priority="36" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40:M40">
-    <cfRule type="cellIs" dxfId="57" priority="35" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="61" priority="35" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D43:D44 G43:G44 J43:K44">
-    <cfRule type="cellIs" dxfId="56" priority="33" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="60" priority="33" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32:M45 C2:M18 C23:M24 C26:M30 C25:D25 F25:M25 G22:M22 C19:D22 F19:M21 K31:M31 I31">
-    <cfRule type="cellIs" dxfId="55" priority="30" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="59" priority="30" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="31" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="58" priority="31" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="32" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="57" priority="32" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N4 N19:N23 N6:N17 N25:N36 N42:N45">
-    <cfRule type="cellIs" dxfId="52" priority="24" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="56" priority="24" operator="greaterThan">
       <formula>$B2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="29" operator="equal">
       <formula>$B2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46">
-    <cfRule type="cellIs" dxfId="50" priority="26" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="54" priority="26" operator="greaterThan">
       <formula>3.66666666666667</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="28" operator="equal">
       <formula>3.66666666666667</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:M46">
-    <cfRule type="cellIs" dxfId="48" priority="25" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="52" priority="25" operator="greaterThan">
       <formula>0.333333333333333</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="27" operator="equal">
       <formula>0.333333333333333</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N38:N40">
-    <cfRule type="cellIs" dxfId="46" priority="22" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="50" priority="22" operator="greaterThan">
       <formula>$B38</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="23" operator="equal">
       <formula>$B38</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L41 I41 G41 E41 C41">
-    <cfRule type="cellIs" dxfId="44" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="48" priority="9" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41:M41">
-    <cfRule type="cellIs" dxfId="43" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="47" priority="8" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31 E31 G31 L31">
-    <cfRule type="cellIs" dxfId="42" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="46" priority="7" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31:H31">
-    <cfRule type="cellIs" dxfId="41" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="45" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31:H31">
-    <cfRule type="cellIs" dxfId="40" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="44" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="43" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="42" priority="5" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2506,8 +2539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3129,13 +3162,13 @@
       <c r="F25" s="14">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="G25" s="14"/>
+      <c r="G25" s="15"/>
       <c r="H25" s="15"/>
-      <c r="I25" s="14"/>
+      <c r="I25" s="15"/>
       <c r="J25" s="15"/>
       <c r="K25" s="15"/>
-      <c r="L25" s="14"/>
-      <c r="M25" s="16"/>
+      <c r="L25" s="15"/>
+      <c r="M25" s="15"/>
       <c r="N25" s="11">
         <f t="shared" si="0"/>
         <v>4.1666666666666664E-2</v>
@@ -3154,13 +3187,13 @@
       <c r="F26" s="15">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="G26" s="14"/>
+      <c r="G26" s="15"/>
       <c r="H26" s="15"/>
-      <c r="I26" s="14"/>
+      <c r="I26" s="15"/>
       <c r="J26" s="15"/>
       <c r="K26" s="15"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="16"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="15"/>
       <c r="N26" s="11">
         <f t="shared" si="0"/>
         <v>2.0833333333333332E-2</v>
@@ -3177,16 +3210,18 @@
       <c r="D27" s="15"/>
       <c r="E27" s="31"/>
       <c r="F27" s="15"/>
-      <c r="G27" s="14"/>
+      <c r="G27" s="15">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="H27" s="15"/>
-      <c r="I27" s="14"/>
+      <c r="I27" s="15"/>
       <c r="J27" s="15"/>
       <c r="K27" s="15"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="16"/>
+      <c r="L27" s="15"/>
+      <c r="M27" s="15"/>
       <c r="N27" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -3200,16 +3235,18 @@
       <c r="D28" s="15"/>
       <c r="E28" s="31"/>
       <c r="F28" s="15"/>
-      <c r="G28" s="14"/>
+      <c r="G28" s="15">
+        <v>6.25E-2</v>
+      </c>
       <c r="H28" s="15"/>
-      <c r="I28" s="14"/>
+      <c r="I28" s="15"/>
       <c r="J28" s="15"/>
       <c r="K28" s="15"/>
-      <c r="L28" s="14"/>
-      <c r="M28" s="16"/>
+      <c r="L28" s="15"/>
+      <c r="M28" s="15"/>
       <c r="N28" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -3223,16 +3260,18 @@
       <c r="D29" s="15"/>
       <c r="E29" s="31"/>
       <c r="F29" s="15"/>
-      <c r="G29" s="14"/>
+      <c r="G29" s="15">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="H29" s="15"/>
-      <c r="I29" s="14"/>
+      <c r="I29" s="15"/>
       <c r="J29" s="15"/>
       <c r="K29" s="15"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="16"/>
+      <c r="L29" s="15"/>
+      <c r="M29" s="15"/>
       <c r="N29" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -3246,16 +3285,18 @@
       <c r="D30" s="15"/>
       <c r="E30" s="31"/>
       <c r="F30" s="15"/>
-      <c r="G30" s="14"/>
+      <c r="G30" s="15">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="H30" s="15"/>
-      <c r="I30" s="14"/>
+      <c r="I30" s="15"/>
       <c r="J30" s="15"/>
       <c r="K30" s="15"/>
-      <c r="L30" s="14"/>
-      <c r="M30" s="16"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="15"/>
       <c r="N30" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
@@ -3269,15 +3310,18 @@
       <c r="D31" s="15"/>
       <c r="E31" s="31"/>
       <c r="F31" s="15"/>
-      <c r="G31" s="14"/>
+      <c r="G31" s="15">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="H31" s="15"/>
       <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
       <c r="K31" s="15"/>
-      <c r="L31" s="14"/>
-      <c r="M31" s="16"/>
+      <c r="L31" s="15"/>
+      <c r="M31" s="15"/>
       <c r="N31" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
@@ -3291,16 +3335,18 @@
       <c r="D32" s="15"/>
       <c r="E32" s="31"/>
       <c r="F32" s="15"/>
-      <c r="G32" s="14"/>
+      <c r="G32" s="15">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="H32" s="15"/>
-      <c r="I32" s="14"/>
+      <c r="I32" s="15"/>
       <c r="J32" s="15"/>
       <c r="K32" s="15"/>
-      <c r="L32" s="14"/>
-      <c r="M32" s="16"/>
+      <c r="L32" s="15"/>
+      <c r="M32" s="15"/>
       <c r="N32" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
@@ -3314,16 +3360,18 @@
       <c r="D33" s="15"/>
       <c r="E33" s="31"/>
       <c r="F33" s="15"/>
-      <c r="G33" s="14"/>
+      <c r="G33" s="15">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="H33" s="15"/>
-      <c r="I33" s="14"/>
+      <c r="I33" s="15"/>
       <c r="J33" s="15"/>
       <c r="K33" s="15"/>
-      <c r="L33" s="14"/>
-      <c r="M33" s="16"/>
+      <c r="L33" s="15"/>
+      <c r="M33" s="15"/>
       <c r="N33" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
@@ -3337,16 +3385,18 @@
       <c r="D34" s="15"/>
       <c r="E34" s="31"/>
       <c r="F34" s="15"/>
-      <c r="G34" s="14"/>
+      <c r="G34" s="15">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="H34" s="15"/>
-      <c r="I34" s="14"/>
+      <c r="I34" s="15"/>
       <c r="J34" s="15"/>
       <c r="K34" s="15"/>
-      <c r="L34" s="14"/>
-      <c r="M34" s="16"/>
+      <c r="L34" s="15"/>
+      <c r="M34" s="15"/>
       <c r="N34" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
@@ -3360,13 +3410,13 @@
       <c r="D35" s="15"/>
       <c r="E35" s="31"/>
       <c r="F35" s="15"/>
-      <c r="G35" s="14"/>
+      <c r="G35" s="15"/>
       <c r="H35" s="15"/>
-      <c r="I35" s="14"/>
+      <c r="I35" s="15"/>
       <c r="J35" s="15"/>
       <c r="K35" s="15"/>
-      <c r="L35" s="14"/>
-      <c r="M35" s="16"/>
+      <c r="L35" s="15"/>
+      <c r="M35" s="15"/>
       <c r="N35" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3383,13 +3433,13 @@
       <c r="D36" s="15"/>
       <c r="E36" s="31"/>
       <c r="F36" s="15"/>
-      <c r="G36" s="14"/>
+      <c r="G36" s="15"/>
       <c r="H36" s="15"/>
-      <c r="I36" s="14"/>
+      <c r="I36" s="15"/>
       <c r="J36" s="15"/>
       <c r="K36" s="15"/>
-      <c r="L36" s="14"/>
-      <c r="M36" s="16"/>
+      <c r="L36" s="15"/>
+      <c r="M36" s="15"/>
       <c r="N36" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3404,13 +3454,13 @@
       <c r="D37" s="15"/>
       <c r="E37" s="31"/>
       <c r="F37" s="15"/>
-      <c r="G37" s="14"/>
+      <c r="G37" s="15"/>
       <c r="H37" s="15"/>
-      <c r="I37" s="14"/>
+      <c r="I37" s="15"/>
       <c r="J37" s="15"/>
       <c r="K37" s="15"/>
-      <c r="L37" s="14"/>
-      <c r="M37" s="16"/>
+      <c r="L37" s="15"/>
+      <c r="M37" s="15"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="22" t="s">
@@ -3425,16 +3475,18 @@
       <c r="F38" s="15">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="G38" s="14"/>
+      <c r="G38" s="15">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="H38" s="15"/>
-      <c r="I38" s="14"/>
+      <c r="I38" s="15"/>
       <c r="J38" s="15"/>
       <c r="K38" s="15"/>
-      <c r="L38" s="14"/>
-      <c r="M38" s="16"/>
+      <c r="L38" s="15"/>
+      <c r="M38" s="15"/>
       <c r="N38" s="11">
         <f t="shared" si="0"/>
-        <v>8.3333333333333329E-2</v>
+        <v>0.10416666666666666</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
@@ -3450,13 +3502,13 @@
       <c r="F39" s="15">
         <v>0.10416666666666667</v>
       </c>
-      <c r="G39" s="14"/>
+      <c r="G39" s="15"/>
       <c r="H39" s="15"/>
-      <c r="I39" s="14"/>
+      <c r="I39" s="15"/>
       <c r="J39" s="15"/>
       <c r="K39" s="15"/>
-      <c r="L39" s="14"/>
-      <c r="M39" s="16"/>
+      <c r="L39" s="15"/>
+      <c r="M39" s="15"/>
       <c r="N39" s="11">
         <f t="shared" si="0"/>
         <v>0.10416666666666667</v>
@@ -3473,13 +3525,13 @@
       <c r="D40" s="15"/>
       <c r="E40" s="31"/>
       <c r="F40" s="15"/>
-      <c r="G40" s="14"/>
+      <c r="G40" s="15"/>
       <c r="H40" s="15"/>
-      <c r="I40" s="14"/>
+      <c r="I40" s="15"/>
       <c r="J40" s="15"/>
       <c r="K40" s="15"/>
-      <c r="L40" s="14"/>
-      <c r="M40" s="16"/>
+      <c r="L40" s="15"/>
+      <c r="M40" s="15"/>
       <c r="N40" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3494,13 +3546,13 @@
       <c r="D41" s="15"/>
       <c r="E41" s="31"/>
       <c r="F41" s="15"/>
-      <c r="G41" s="14"/>
+      <c r="G41" s="15"/>
       <c r="H41" s="15"/>
-      <c r="I41" s="14"/>
+      <c r="I41" s="15"/>
       <c r="J41" s="15"/>
       <c r="K41" s="15"/>
-      <c r="L41" s="14"/>
-      <c r="M41" s="16"/>
+      <c r="L41" s="15"/>
+      <c r="M41" s="15"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="22" t="s">
@@ -3521,16 +3573,18 @@
       <c r="F42" s="15">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="G42" s="15"/>
+      <c r="G42" s="15">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="H42" s="15"/>
       <c r="I42" s="15"/>
       <c r="J42" s="15"/>
       <c r="K42" s="15"/>
       <c r="L42" s="15"/>
-      <c r="M42" s="16"/>
+      <c r="M42" s="15"/>
       <c r="N42" s="11">
         <f t="shared" si="0"/>
-        <v>0.3125</v>
+        <v>0.35416666666666669</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
@@ -3544,13 +3598,13 @@
       <c r="D43" s="14"/>
       <c r="E43" s="31"/>
       <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="14"/>
-      <c r="K43" s="14"/>
-      <c r="L43" s="14"/>
-      <c r="M43" s="16"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="15"/>
+      <c r="I43" s="15"/>
+      <c r="J43" s="15"/>
+      <c r="K43" s="15"/>
+      <c r="L43" s="15"/>
+      <c r="M43" s="15"/>
       <c r="N43" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3621,7 +3675,7 @@
       </c>
       <c r="G46" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333337</v>
       </c>
       <c r="H46" s="11">
         <f t="shared" si="1"/>
@@ -3651,166 +3705,182 @@
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M47" s="11">
         <f>SUM(C46:M46)</f>
-        <v>1.3333333333333333</v>
+        <v>1.6666666666666665</v>
       </c>
       <c r="N47" s="11">
         <f>SUM(N2:N45)</f>
-        <v>1.3333333333333335</v>
+        <v>1.6666666666666667</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:M2 F43:F44 H43:I44 I32:I42 C3:C30 I3:I30 L3:L30 F25 G3:G30 E3:E18 F19:F21 I45 C32:C45 E45 G32:G45 L32:L45">
-    <cfRule type="cellIs" dxfId="37" priority="44" operator="greaterThan">
+  <conditionalFormatting sqref="C2:M2 F43:F44 H44:I44 C3:C30 I3:I24 L3:L24 F25 G3:G24 E3:E18 F19:F21 I45 C32:C45 E45 G44:G45 L44:L45">
+    <cfRule type="cellIs" dxfId="41" priority="48" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:M2 C45:M45 C4:M18 C23:D30 C19:D21 F19:M21 K31:M31 I31 F23:M30 C32:D44 F32:M44">
-    <cfRule type="cellIs" dxfId="36" priority="43" operator="greaterThan">
+  <conditionalFormatting sqref="C2:M2 C45:M45 C4:M18 C23:D30 C19:D21 F19:M21 F23:M24 C32:D44 F44:M44 F32:F43 F25:F30">
+    <cfRule type="cellIs" dxfId="40" priority="47" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L40 I40 G40 C40">
-    <cfRule type="cellIs" dxfId="35" priority="42" operator="greaterThan">
+  <conditionalFormatting sqref="C40">
+    <cfRule type="cellIs" dxfId="39" priority="46" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C40:D40 F40:M40">
-    <cfRule type="cellIs" dxfId="34" priority="41" operator="greaterThan">
+  <conditionalFormatting sqref="C40:D40 F40">
+    <cfRule type="cellIs" dxfId="38" priority="45" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D43:D44 G43:G44 J43:K44">
-    <cfRule type="cellIs" dxfId="33" priority="39" operator="greaterThan">
+  <conditionalFormatting sqref="D43:D44 G44 J44:K44">
+    <cfRule type="cellIs" dxfId="37" priority="43" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C45:M45 C2:M18 G22:M22 C19:D30 F19:M21 K31:M31 I31 F23:M30 C32:D44 F32:M44">
-    <cfRule type="cellIs" dxfId="32" priority="36" operator="greaterThan">
+  <conditionalFormatting sqref="C45:M45 C2:M18 G22:M22 C19:D30 F19:M21 F23:M24 C32:D44 F44:M44 F32:F43 F25:F30">
+    <cfRule type="cellIs" dxfId="36" priority="40" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="37" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="41" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="38" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="34" priority="42" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N4 N19:N23 N6:N17 N25:N36 N42:N45">
-    <cfRule type="cellIs" dxfId="29" priority="30" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="34" operator="greaterThan">
       <formula>$B2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="39" operator="equal">
       <formula>$B2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46">
+    <cfRule type="cellIs" dxfId="31" priority="36" operator="greaterThan">
+      <formula>3.66666666666667</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="38" operator="equal">
+      <formula>3.66666666666667</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C46:M46">
+    <cfRule type="cellIs" dxfId="29" priority="35" operator="greaterThan">
+      <formula>0.333333333333333</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="37" operator="equal">
+      <formula>0.333333333333333</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N38:N40">
     <cfRule type="cellIs" dxfId="27" priority="32" operator="greaterThan">
-      <formula>3.66666666666667</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="34" operator="equal">
-      <formula>3.66666666666667</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C46:M46">
-    <cfRule type="cellIs" dxfId="25" priority="31" operator="greaterThan">
-      <formula>0.333333333333333</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="33" operator="equal">
-      <formula>0.333333333333333</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N38:N40">
-    <cfRule type="cellIs" dxfId="23" priority="28" operator="greaterThan">
       <formula>$B38</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="33" operator="equal">
       <formula>$B38</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L41 I41 G41 C41">
-    <cfRule type="cellIs" dxfId="21" priority="22" operator="greaterThan">
+  <conditionalFormatting sqref="C41">
+    <cfRule type="cellIs" dxfId="25" priority="26" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C41:D41 F41:M41">
+  <conditionalFormatting sqref="C41:D41 F41">
+    <cfRule type="cellIs" dxfId="24" priority="25" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C31">
+    <cfRule type="cellIs" dxfId="23" priority="24" operator="greaterThan">
+      <formula>0.0000115740740740741</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C31:D31 F31">
+    <cfRule type="cellIs" dxfId="22" priority="23" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C31:D31 F31">
+    <cfRule type="cellIs" dxfId="21" priority="20" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
     <cfRule type="cellIs" dxfId="20" priority="21" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C31 G31 L31">
-    <cfRule type="cellIs" dxfId="19" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="22" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E19">
+    <cfRule type="cellIs" dxfId="18" priority="19" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C31:D31 F31:H31">
-    <cfRule type="cellIs" dxfId="18" priority="19" operator="greaterThan">
+  <conditionalFormatting sqref="E19">
+    <cfRule type="cellIs" dxfId="17" priority="18" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C31:D31 F31:H31">
-    <cfRule type="cellIs" dxfId="17" priority="16" operator="greaterThan">
+  <conditionalFormatting sqref="E19">
+    <cfRule type="cellIs" dxfId="16" priority="15" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="16" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="17" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E19">
-    <cfRule type="cellIs" dxfId="14" priority="15" operator="greaterThan">
+  <conditionalFormatting sqref="E20:E44">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E19">
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="greaterThan">
+  <conditionalFormatting sqref="E20:E44">
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E19">
-    <cfRule type="cellIs" dxfId="12" priority="11" operator="greaterThan">
+  <conditionalFormatting sqref="E20:E44">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E20:E44">
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="greaterThan">
+  <conditionalFormatting sqref="F22">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="greaterThan">
       <formula>0.0000115740740740741</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E20:E44">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="greaterThan">
+  <conditionalFormatting sqref="F22">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E20:E44">
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="greaterThan">
+  <conditionalFormatting sqref="F22">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F22">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
-      <formula>0.0000115740740740741</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F22">
+  <conditionalFormatting sqref="G25:M43">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F22">
+  <conditionalFormatting sqref="G25:M43">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Jour 6 - Finition du site
</commit_message>
<xml_diff>
--- a/docs/Analysis/RP_Planification.xlsx
+++ b/docs/Analysis/RP_Planification.xlsx
@@ -2552,7 +2552,7 @@
   <dimension ref="A1:N47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3427,16 +3427,18 @@
       <c r="F35" s="15"/>
       <c r="G35" s="15"/>
       <c r="H35" s="15">
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="I35" s="15"/>
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="I35" s="15">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="J35" s="15"/>
       <c r="K35" s="15"/>
       <c r="L35" s="15"/>
       <c r="M35" s="15"/>
       <c r="N35" s="11">
         <f t="shared" si="0"/>
-        <v>4.1666666666666664E-2</v>
+        <v>0.10416666666666666</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
@@ -3499,16 +3501,18 @@
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="H38" s="15">
-        <v>0.125</v>
-      </c>
-      <c r="I38" s="15"/>
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="I38" s="15">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="J38" s="15"/>
       <c r="K38" s="15"/>
       <c r="L38" s="15"/>
       <c r="M38" s="15"/>
       <c r="N38" s="11">
         <f t="shared" si="0"/>
-        <v>0.22916666666666666</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
@@ -3526,14 +3530,16 @@
       </c>
       <c r="G39" s="15"/>
       <c r="H39" s="15"/>
-      <c r="I39" s="15"/>
+      <c r="I39" s="15">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="J39" s="15"/>
       <c r="K39" s="15"/>
       <c r="L39" s="15"/>
       <c r="M39" s="15"/>
       <c r="N39" s="11">
         <f t="shared" si="0"/>
-        <v>0.10416666666666667</v>
+        <v>0.1875</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
@@ -3602,14 +3608,16 @@
       <c r="H42" s="15">
         <v>0.125</v>
       </c>
-      <c r="I42" s="15"/>
+      <c r="I42" s="15">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="J42" s="15"/>
       <c r="K42" s="15"/>
       <c r="L42" s="15"/>
       <c r="M42" s="15"/>
       <c r="N42" s="11">
         <f t="shared" si="0"/>
-        <v>0.47916666666666669</v>
+        <v>0.5625</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
@@ -3704,11 +3712,11 @@
       </c>
       <c r="H46" s="11">
         <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
+        <v>0.33333333333333337</v>
       </c>
       <c r="I46" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="J46" s="11">
         <f t="shared" si="1"/>
@@ -3730,11 +3738,11 @@
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M47" s="11">
         <f>SUM(C46:M46)</f>
-        <v>1.9999999999999998</v>
+        <v>2.3333333333333335</v>
       </c>
       <c r="N47" s="11">
         <f>SUM(N2:N45)</f>
-        <v>2</v>
+        <v>2.333333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Avancement de la documentation et du design du site
</commit_message>
<xml_diff>
--- a/docs/Analysis/RP_Planification.xlsx
+++ b/docs/Analysis/RP_Planification.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="57">
   <si>
     <t>Tâches à réaliser</t>
   </si>
@@ -193,6 +193,9 @@
   </si>
   <si>
     <t>Évaluation d'une annonce</t>
+  </si>
+  <si>
+    <t>Manuel utilisateur</t>
   </si>
 </sst>
 </file>
@@ -2552,7 +2555,7 @@
   <dimension ref="A1:N47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+      <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3533,13 +3536,15 @@
       <c r="I39" s="15">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="J39" s="15"/>
+      <c r="J39" s="15">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="K39" s="15"/>
       <c r="L39" s="15"/>
       <c r="M39" s="15"/>
       <c r="N39" s="11">
         <f t="shared" si="0"/>
-        <v>0.1875</v>
+        <v>0.27083333333333331</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
@@ -3611,18 +3616,20 @@
       <c r="I42" s="15">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="J42" s="15"/>
+      <c r="J42" s="15">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="K42" s="15"/>
       <c r="L42" s="15"/>
       <c r="M42" s="15"/>
       <c r="N42" s="11">
         <f t="shared" si="0"/>
-        <v>0.5625</v>
+        <v>0.64583333333333337</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="22" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="B43" s="13">
         <v>0.33333333333333331</v>
@@ -3634,13 +3641,15 @@
       <c r="G43" s="15"/>
       <c r="H43" s="15"/>
       <c r="I43" s="15"/>
-      <c r="J43" s="15"/>
+      <c r="J43" s="15">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="K43" s="15"/>
       <c r="L43" s="15"/>
       <c r="M43" s="15"/>
       <c r="N43" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
@@ -3720,7 +3729,7 @@
       </c>
       <c r="J46" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="K46" s="11">
         <f t="shared" si="1"/>
@@ -3738,11 +3747,11 @@
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M47" s="11">
         <f>SUM(C46:M46)</f>
-        <v>2.3333333333333335</v>
+        <v>2.666666666666667</v>
       </c>
       <c r="N47" s="11">
         <f>SUM(N2:N45)</f>
-        <v>2.333333333333333</v>
+        <v>2.6666666666666665</v>
       </c>
     </row>
   </sheetData>

</xml_diff>